<commit_message>
Badania 1 czesc skonczona
</commit_message>
<xml_diff>
--- a/doc/Wyniki_end.xlsx
+++ b/doc/Wyniki_end.xlsx
@@ -344,12 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,6 +355,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M82" workbookViewId="0">
-      <selection activeCell="Y88" sqref="Y88"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4:AF18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -674,218 +674,218 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
     </row>
     <row r="2" spans="1:32">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18"/>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="18"/>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
       <c r="L4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
       <c r="W4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X4" s="19" t="s">
+      <c r="X4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="21"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
       <c r="L5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
       <c r="W5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="19" t="s">
+      <c r="X5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="20"/>
-      <c r="AD5" s="20"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="21"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17" t="s">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17" t="s">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17" t="s">
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
       <c r="W6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X6" s="19" t="s">
+      <c r="X6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="19" t="s">
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB6" s="20"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="19" t="s">
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE6" s="20"/>
-      <c r="AF6" s="21"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32">
       <c r="B7" s="1" t="s">
@@ -1334,7 +1334,7 @@
         <v>53.02</v>
       </c>
       <c r="AE11" s="1">
-        <v>16700</v>
+        <v>15700</v>
       </c>
       <c r="AF11" s="1">
         <v>272</v>
@@ -1610,7 +1610,7 @@
         <v>42.06</v>
       </c>
       <c r="AE14" s="1">
-        <v>17066</v>
+        <v>16066</v>
       </c>
       <c r="AF14" s="1">
         <v>272</v>
@@ -1702,7 +1702,7 @@
         <v>43.21</v>
       </c>
       <c r="AE15" s="1">
-        <v>17260</v>
+        <v>16260</v>
       </c>
       <c r="AF15" s="1">
         <v>275</v>
@@ -1794,7 +1794,7 @@
         <v>46.05</v>
       </c>
       <c r="AE16" s="1">
-        <v>17249</v>
+        <v>16249</v>
       </c>
       <c r="AF16" s="1">
         <v>273</v>
@@ -1886,7 +1886,7 @@
         <v>45.05</v>
       </c>
       <c r="AE17" s="1">
-        <v>17214</v>
+        <v>16214</v>
       </c>
       <c r="AF17" s="1">
         <v>277</v>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AE18" s="12">
         <f t="shared" si="2"/>
-        <v>16482</v>
+        <v>15982</v>
       </c>
       <c r="AF18" s="12">
         <f t="shared" si="2"/>
@@ -2015,145 +2015,145 @@
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="19"/>
       <c r="L22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="19" t="s">
+      <c r="M22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="21"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="19"/>
       <c r="W22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X22" s="19" t="s">
+      <c r="X22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-      <c r="AA22" s="20"/>
-      <c r="AB22" s="20"/>
-      <c r="AC22" s="20"/>
-      <c r="AD22" s="20"/>
-      <c r="AE22" s="20"/>
-      <c r="AF22" s="21"/>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
+      <c r="AA22" s="18"/>
+      <c r="AB22" s="18"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="18"/>
+      <c r="AE22" s="18"/>
+      <c r="AF22" s="19"/>
     </row>
     <row r="23" spans="1:32">
       <c r="A23" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
       <c r="L23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M23" s="19" t="s">
+      <c r="M23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="21"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="19"/>
       <c r="W23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X23" s="19" t="s">
+      <c r="X23" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Y23" s="20"/>
-      <c r="Z23" s="20"/>
-      <c r="AA23" s="20"/>
-      <c r="AB23" s="20"/>
-      <c r="AC23" s="20"/>
-      <c r="AD23" s="20"/>
-      <c r="AE23" s="20"/>
-      <c r="AF23" s="21"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+      <c r="AA23" s="18"/>
+      <c r="AB23" s="18"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="18"/>
+      <c r="AE23" s="18"/>
+      <c r="AF23" s="19"/>
     </row>
     <row r="24" spans="1:32">
       <c r="A24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="19" t="s">
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="19" t="s">
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="22"/>
-      <c r="J24" s="23"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="21"/>
       <c r="L24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N24" s="20"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="19" t="s">
+      <c r="N24" s="18"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="17" t="s">
+      <c r="Q24" s="18"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
       <c r="W24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X24" s="19" t="s">
+      <c r="X24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y24" s="20"/>
-      <c r="Z24" s="21"/>
-      <c r="AA24" s="19" t="s">
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB24" s="20"/>
-      <c r="AC24" s="21"/>
-      <c r="AD24" s="19" t="s">
+      <c r="AB24" s="18"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE24" s="20"/>
-      <c r="AF24" s="21"/>
+      <c r="AE24" s="18"/>
+      <c r="AF24" s="19"/>
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="9"/>
@@ -2334,218 +2334,218 @@
       </c>
     </row>
     <row r="28" spans="1:32">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="18"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="18"/>
-      <c r="U28" s="18"/>
-      <c r="V28" s="18"/>
-      <c r="W28" s="18"/>
-      <c r="X28" s="18"/>
-      <c r="Y28" s="18"/>
-      <c r="Z28" s="18"/>
-      <c r="AA28" s="18"/>
-      <c r="AB28" s="18"/>
-      <c r="AC28" s="18"/>
-      <c r="AD28" s="18"/>
-      <c r="AE28" s="18"/>
-      <c r="AF28" s="18"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="S28" s="23"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+      <c r="AA28" s="23"/>
+      <c r="AB28" s="23"/>
+      <c r="AC28" s="23"/>
+      <c r="AD28" s="23"/>
+      <c r="AE28" s="23"/>
+      <c r="AF28" s="23"/>
     </row>
     <row r="29" spans="1:32">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="18"/>
-      <c r="Y29" s="18"/>
-      <c r="Z29" s="18"/>
-      <c r="AA29" s="18"/>
-      <c r="AB29" s="18"/>
-      <c r="AC29" s="18"/>
-      <c r="AD29" s="18"/>
-      <c r="AE29" s="18"/>
-      <c r="AF29" s="18"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
+      <c r="S29" s="23"/>
+      <c r="T29" s="23"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+      <c r="AA29" s="23"/>
+      <c r="AB29" s="23"/>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="23"/>
+      <c r="AE29" s="23"/>
+      <c r="AF29" s="23"/>
     </row>
     <row r="31" spans="1:32">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
       <c r="L31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M31" s="17" t="s">
+      <c r="M31" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="17"/>
+      <c r="N31" s="22"/>
+      <c r="O31" s="22"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
       <c r="W31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X31" s="17" t="s">
+      <c r="X31" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Y31" s="17"/>
-      <c r="Z31" s="17"/>
-      <c r="AA31" s="17"/>
-      <c r="AB31" s="17"/>
-      <c r="AC31" s="17"/>
-      <c r="AD31" s="17"/>
-      <c r="AE31" s="17"/>
-      <c r="AF31" s="17"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+      <c r="AA31" s="22"/>
+      <c r="AB31" s="22"/>
+      <c r="AC31" s="22"/>
+      <c r="AD31" s="22"/>
+      <c r="AE31" s="22"/>
+      <c r="AF31" s="22"/>
     </row>
     <row r="32" spans="1:32">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
       <c r="L32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M32" s="17" t="s">
+      <c r="M32" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="22"/>
       <c r="W32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X32" s="17" t="s">
+      <c r="X32" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="Y32" s="17"/>
-      <c r="Z32" s="17"/>
-      <c r="AA32" s="17"/>
-      <c r="AB32" s="17"/>
-      <c r="AC32" s="17"/>
-      <c r="AD32" s="17"/>
-      <c r="AE32" s="17"/>
-      <c r="AF32" s="17"/>
+      <c r="Y32" s="22"/>
+      <c r="Z32" s="22"/>
+      <c r="AA32" s="22"/>
+      <c r="AB32" s="22"/>
+      <c r="AC32" s="22"/>
+      <c r="AD32" s="22"/>
+      <c r="AE32" s="22"/>
+      <c r="AF32" s="22"/>
     </row>
     <row r="33" spans="1:32">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17" t="s">
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17" t="s">
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
       <c r="L33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="17" t="s">
+      <c r="M33" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N33" s="17"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="17" t="s">
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17" t="s">
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
+      <c r="S33" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T33" s="17"/>
-      <c r="U33" s="17"/>
+      <c r="T33" s="22"/>
+      <c r="U33" s="22"/>
       <c r="W33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X33" s="17" t="s">
+      <c r="X33" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y33" s="17"/>
-      <c r="Z33" s="17"/>
-      <c r="AA33" s="17" t="s">
+      <c r="Y33" s="22"/>
+      <c r="Z33" s="22"/>
+      <c r="AA33" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB33" s="17"/>
-      <c r="AC33" s="17"/>
-      <c r="AD33" s="17" t="s">
+      <c r="AB33" s="22"/>
+      <c r="AC33" s="22"/>
+      <c r="AD33" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AE33" s="17"/>
-      <c r="AF33" s="17"/>
+      <c r="AE33" s="22"/>
+      <c r="AF33" s="22"/>
     </row>
     <row r="34" spans="1:32">
       <c r="B34" s="1" t="s">
@@ -2889,7 +2889,7 @@
         <v>466</v>
       </c>
       <c r="AA37" s="1">
-        <v>63.93</v>
+        <v>73.930000000000007</v>
       </c>
       <c r="AB37" s="1">
         <v>28172</v>
@@ -3073,7 +3073,7 @@
         <v>472</v>
       </c>
       <c r="AA39" s="1">
-        <v>50.89</v>
+        <v>70.89</v>
       </c>
       <c r="AB39" s="1">
         <v>28984</v>
@@ -3165,7 +3165,7 @@
         <v>476</v>
       </c>
       <c r="AA40" s="1">
-        <v>40.92</v>
+        <v>80.92</v>
       </c>
       <c r="AB40" s="1">
         <v>28910</v>
@@ -3349,7 +3349,7 @@
         <v>485</v>
       </c>
       <c r="AA42" s="1">
-        <v>58.04</v>
+        <v>78.040000000000006</v>
       </c>
       <c r="AB42" s="1">
         <v>30025</v>
@@ -3545,7 +3545,7 @@
         <v>47.04</v>
       </c>
       <c r="AE44" s="1">
-        <v>24084</v>
+        <v>22084</v>
       </c>
       <c r="AF44" s="1">
         <v>488</v>
@@ -3647,7 +3647,7 @@
       </c>
       <c r="AA45" s="12">
         <f>AVERAGE(AA36:AA44)</f>
-        <v>68.484444444444449</v>
+        <v>78.484444444444435</v>
       </c>
       <c r="AB45" s="12">
         <f t="shared" si="5"/>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="AE45" s="12">
         <f t="shared" si="5"/>
-        <v>22083.3</v>
+        <v>21883.3</v>
       </c>
       <c r="AF45" s="12">
         <f>AVERAGE(AF35:AF44)</f>
@@ -3674,145 +3674,145 @@
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
       <c r="L49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M49" s="17" t="s">
+      <c r="M49" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N49" s="17"/>
-      <c r="O49" s="17"/>
-      <c r="P49" s="17"/>
-      <c r="Q49" s="17"/>
-      <c r="R49" s="17"/>
-      <c r="S49" s="17"/>
-      <c r="T49" s="17"/>
-      <c r="U49" s="17"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
+      <c r="P49" s="22"/>
+      <c r="Q49" s="22"/>
+      <c r="R49" s="22"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="22"/>
+      <c r="U49" s="22"/>
       <c r="W49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X49" s="17" t="s">
+      <c r="X49" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Y49" s="17"/>
-      <c r="Z49" s="17"/>
-      <c r="AA49" s="17"/>
-      <c r="AB49" s="17"/>
-      <c r="AC49" s="17"/>
-      <c r="AD49" s="17"/>
-      <c r="AE49" s="17"/>
-      <c r="AF49" s="17"/>
+      <c r="Y49" s="22"/>
+      <c r="Z49" s="22"/>
+      <c r="AA49" s="22"/>
+      <c r="AB49" s="22"/>
+      <c r="AC49" s="22"/>
+      <c r="AD49" s="22"/>
+      <c r="AE49" s="22"/>
+      <c r="AF49" s="22"/>
     </row>
     <row r="50" spans="1:32">
       <c r="A50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="17"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
       <c r="L50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M50" s="17" t="s">
+      <c r="M50" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="N50" s="17"/>
-      <c r="O50" s="17"/>
-      <c r="P50" s="17"/>
-      <c r="Q50" s="17"/>
-      <c r="R50" s="17"/>
-      <c r="S50" s="17"/>
-      <c r="T50" s="17"/>
-      <c r="U50" s="17"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="22"/>
+      <c r="S50" s="22"/>
+      <c r="T50" s="22"/>
+      <c r="U50" s="22"/>
       <c r="W50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X50" s="17" t="s">
+      <c r="X50" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Y50" s="17"/>
-      <c r="Z50" s="17"/>
-      <c r="AA50" s="17"/>
-      <c r="AB50" s="17"/>
-      <c r="AC50" s="17"/>
-      <c r="AD50" s="17"/>
-      <c r="AE50" s="17"/>
-      <c r="AF50" s="17"/>
+      <c r="Y50" s="22"/>
+      <c r="Z50" s="22"/>
+      <c r="AA50" s="22"/>
+      <c r="AB50" s="22"/>
+      <c r="AC50" s="22"/>
+      <c r="AD50" s="22"/>
+      <c r="AE50" s="22"/>
+      <c r="AF50" s="22"/>
     </row>
     <row r="51" spans="1:32">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17" t="s">
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17" t="s">
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
       <c r="L51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M51" s="17" t="s">
+      <c r="M51" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N51" s="17"/>
-      <c r="O51" s="17"/>
-      <c r="P51" s="17" t="s">
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Q51" s="17"/>
-      <c r="R51" s="17"/>
-      <c r="S51" s="17" t="s">
+      <c r="Q51" s="22"/>
+      <c r="R51" s="22"/>
+      <c r="S51" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T51" s="17"/>
-      <c r="U51" s="17"/>
+      <c r="T51" s="22"/>
+      <c r="U51" s="22"/>
       <c r="W51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X51" s="17" t="s">
+      <c r="X51" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y51" s="17"/>
-      <c r="Z51" s="17"/>
-      <c r="AA51" s="17" t="s">
+      <c r="Y51" s="22"/>
+      <c r="Z51" s="22"/>
+      <c r="AA51" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB51" s="17"/>
-      <c r="AC51" s="17"/>
-      <c r="AD51" s="17" t="s">
+      <c r="AB51" s="22"/>
+      <c r="AC51" s="22"/>
+      <c r="AD51" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AE51" s="17"/>
-      <c r="AF51" s="17"/>
+      <c r="AE51" s="22"/>
+      <c r="AF51" s="22"/>
     </row>
     <row r="52" spans="1:32">
       <c r="A52" s="11"/>
@@ -3917,7 +3917,7 @@
         <v>1.5960000000000001</v>
       </c>
       <c r="F53" s="1">
-        <v>1218</v>
+        <v>1196</v>
       </c>
       <c r="G53" s="1">
         <v>117</v>
@@ -3993,218 +3993,218 @@
       </c>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="18"/>
-      <c r="O55" s="18"/>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="18"/>
-      <c r="U55" s="18"/>
-      <c r="V55" s="18"/>
-      <c r="W55" s="18"/>
-      <c r="X55" s="18"/>
-      <c r="Y55" s="18"/>
-      <c r="Z55" s="18"/>
-      <c r="AA55" s="18"/>
-      <c r="AB55" s="18"/>
-      <c r="AC55" s="18"/>
-      <c r="AD55" s="18"/>
-      <c r="AE55" s="18"/>
-      <c r="AF55" s="18"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="23"/>
+      <c r="N55" s="23"/>
+      <c r="O55" s="23"/>
+      <c r="P55" s="23"/>
+      <c r="Q55" s="23"/>
+      <c r="R55" s="23"/>
+      <c r="S55" s="23"/>
+      <c r="T55" s="23"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="23"/>
+      <c r="W55" s="23"/>
+      <c r="X55" s="23"/>
+      <c r="Y55" s="23"/>
+      <c r="Z55" s="23"/>
+      <c r="AA55" s="23"/>
+      <c r="AB55" s="23"/>
+      <c r="AC55" s="23"/>
+      <c r="AD55" s="23"/>
+      <c r="AE55" s="23"/>
+      <c r="AF55" s="23"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="18"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
-      <c r="N56" s="18"/>
-      <c r="O56" s="18"/>
-      <c r="P56" s="18"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="18"/>
-      <c r="T56" s="18"/>
-      <c r="U56" s="18"/>
-      <c r="V56" s="18"/>
-      <c r="W56" s="18"/>
-      <c r="X56" s="18"/>
-      <c r="Y56" s="18"/>
-      <c r="Z56" s="18"/>
-      <c r="AA56" s="18"/>
-      <c r="AB56" s="18"/>
-      <c r="AC56" s="18"/>
-      <c r="AD56" s="18"/>
-      <c r="AE56" s="18"/>
-      <c r="AF56" s="18"/>
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
+      <c r="K56" s="23"/>
+      <c r="L56" s="23"/>
+      <c r="M56" s="23"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="23"/>
+      <c r="P56" s="23"/>
+      <c r="Q56" s="23"/>
+      <c r="R56" s="23"/>
+      <c r="S56" s="23"/>
+      <c r="T56" s="23"/>
+      <c r="U56" s="23"/>
+      <c r="V56" s="23"/>
+      <c r="W56" s="23"/>
+      <c r="X56" s="23"/>
+      <c r="Y56" s="23"/>
+      <c r="Z56" s="23"/>
+      <c r="AA56" s="23"/>
+      <c r="AB56" s="23"/>
+      <c r="AC56" s="23"/>
+      <c r="AD56" s="23"/>
+      <c r="AE56" s="23"/>
+      <c r="AF56" s="23"/>
     </row>
     <row r="58" spans="1:32">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
-      <c r="J58" s="17"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
       <c r="L58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M58" s="17" t="s">
+      <c r="M58" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N58" s="17"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="17"/>
-      <c r="Q58" s="17"/>
-      <c r="R58" s="17"/>
-      <c r="S58" s="17"/>
-      <c r="T58" s="17"/>
-      <c r="U58" s="17"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="22"/>
+      <c r="T58" s="22"/>
+      <c r="U58" s="22"/>
       <c r="W58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X58" s="17" t="s">
+      <c r="X58" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Y58" s="17"/>
-      <c r="Z58" s="17"/>
-      <c r="AA58" s="17"/>
-      <c r="AB58" s="17"/>
-      <c r="AC58" s="17"/>
-      <c r="AD58" s="17"/>
-      <c r="AE58" s="17"/>
-      <c r="AF58" s="17"/>
+      <c r="Y58" s="22"/>
+      <c r="Z58" s="22"/>
+      <c r="AA58" s="22"/>
+      <c r="AB58" s="22"/>
+      <c r="AC58" s="22"/>
+      <c r="AD58" s="22"/>
+      <c r="AE58" s="22"/>
+      <c r="AF58" s="22"/>
     </row>
     <row r="59" spans="1:32">
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
       <c r="L59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M59" s="17" t="s">
+      <c r="M59" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
-      <c r="P59" s="17"/>
-      <c r="Q59" s="17"/>
-      <c r="R59" s="17"/>
-      <c r="S59" s="17"/>
-      <c r="T59" s="17"/>
-      <c r="U59" s="17"/>
+      <c r="N59" s="22"/>
+      <c r="O59" s="22"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="22"/>
+      <c r="S59" s="22"/>
+      <c r="T59" s="22"/>
+      <c r="U59" s="22"/>
       <c r="W59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X59" s="17" t="s">
+      <c r="X59" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="Y59" s="17"/>
-      <c r="Z59" s="17"/>
-      <c r="AA59" s="17"/>
-      <c r="AB59" s="17"/>
-      <c r="AC59" s="17"/>
-      <c r="AD59" s="17"/>
-      <c r="AE59" s="17"/>
-      <c r="AF59" s="17"/>
+      <c r="Y59" s="22"/>
+      <c r="Z59" s="22"/>
+      <c r="AA59" s="22"/>
+      <c r="AB59" s="22"/>
+      <c r="AC59" s="22"/>
+      <c r="AD59" s="22"/>
+      <c r="AE59" s="22"/>
+      <c r="AF59" s="22"/>
     </row>
     <row r="60" spans="1:32">
       <c r="A60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="19" t="s">
+      <c r="C60" s="18"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="21"/>
-      <c r="H60" s="17" t="s">
+      <c r="F60" s="18"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="17"/>
-      <c r="J60" s="17"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
       <c r="L60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M60" s="19" t="s">
+      <c r="M60" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N60" s="20"/>
-      <c r="O60" s="21"/>
-      <c r="P60" s="19" t="s">
+      <c r="N60" s="18"/>
+      <c r="O60" s="19"/>
+      <c r="P60" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q60" s="20"/>
-      <c r="R60" s="21"/>
-      <c r="S60" s="17" t="s">
+      <c r="Q60" s="18"/>
+      <c r="R60" s="19"/>
+      <c r="S60" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T60" s="17"/>
-      <c r="U60" s="17"/>
+      <c r="T60" s="22"/>
+      <c r="U60" s="22"/>
       <c r="W60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X60" s="17" t="s">
+      <c r="X60" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y60" s="17"/>
-      <c r="Z60" s="17"/>
-      <c r="AA60" s="17" t="s">
+      <c r="Y60" s="22"/>
+      <c r="Z60" s="22"/>
+      <c r="AA60" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB60" s="17"/>
-      <c r="AC60" s="17"/>
-      <c r="AD60" s="17" t="s">
+      <c r="AB60" s="22"/>
+      <c r="AC60" s="22"/>
+      <c r="AD60" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AE60" s="17"/>
-      <c r="AF60" s="17"/>
+      <c r="AE60" s="22"/>
+      <c r="AF60" s="22"/>
     </row>
     <row r="61" spans="1:32">
       <c r="A61" s="11"/>
@@ -5333,145 +5333,145 @@
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
-      <c r="J74" s="17"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
       <c r="L74" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M74" s="17" t="s">
+      <c r="M74" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N74" s="17"/>
-      <c r="O74" s="17"/>
-      <c r="P74" s="17"/>
-      <c r="Q74" s="17"/>
-      <c r="R74" s="17"/>
-      <c r="S74" s="17"/>
-      <c r="T74" s="17"/>
-      <c r="U74" s="17"/>
+      <c r="N74" s="22"/>
+      <c r="O74" s="22"/>
+      <c r="P74" s="22"/>
+      <c r="Q74" s="22"/>
+      <c r="R74" s="22"/>
+      <c r="S74" s="22"/>
+      <c r="T74" s="22"/>
+      <c r="U74" s="22"/>
       <c r="W74" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="X74" s="17" t="s">
+      <c r="X74" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Y74" s="17"/>
-      <c r="Z74" s="17"/>
-      <c r="AA74" s="17"/>
-      <c r="AB74" s="17"/>
-      <c r="AC74" s="17"/>
-      <c r="AD74" s="17"/>
-      <c r="AE74" s="17"/>
-      <c r="AF74" s="17"/>
+      <c r="Y74" s="22"/>
+      <c r="Z74" s="22"/>
+      <c r="AA74" s="22"/>
+      <c r="AB74" s="22"/>
+      <c r="AC74" s="22"/>
+      <c r="AD74" s="22"/>
+      <c r="AE74" s="22"/>
+      <c r="AF74" s="22"/>
     </row>
     <row r="75" spans="1:32">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
-      <c r="J75" s="17"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
       <c r="L75" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M75" s="17" t="s">
+      <c r="M75" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="N75" s="17"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="17"/>
-      <c r="Q75" s="17"/>
-      <c r="R75" s="17"/>
-      <c r="S75" s="17"/>
-      <c r="T75" s="17"/>
-      <c r="U75" s="17"/>
+      <c r="N75" s="22"/>
+      <c r="O75" s="22"/>
+      <c r="P75" s="22"/>
+      <c r="Q75" s="22"/>
+      <c r="R75" s="22"/>
+      <c r="S75" s="22"/>
+      <c r="T75" s="22"/>
+      <c r="U75" s="22"/>
       <c r="W75" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="X75" s="17" t="s">
+      <c r="X75" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Y75" s="17"/>
-      <c r="Z75" s="17"/>
-      <c r="AA75" s="17"/>
-      <c r="AB75" s="17"/>
-      <c r="AC75" s="17"/>
-      <c r="AD75" s="17"/>
-      <c r="AE75" s="17"/>
-      <c r="AF75" s="17"/>
+      <c r="Y75" s="22"/>
+      <c r="Z75" s="22"/>
+      <c r="AA75" s="22"/>
+      <c r="AB75" s="22"/>
+      <c r="AC75" s="22"/>
+      <c r="AD75" s="22"/>
+      <c r="AE75" s="22"/>
+      <c r="AF75" s="22"/>
     </row>
     <row r="76" spans="1:32">
       <c r="A76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="B76" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="20"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="19" t="s">
+      <c r="C76" s="18"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F76" s="20"/>
-      <c r="G76" s="21"/>
-      <c r="H76" s="17" t="s">
+      <c r="F76" s="18"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I76" s="17"/>
-      <c r="J76" s="17"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
       <c r="L76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M76" s="17" t="s">
+      <c r="M76" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N76" s="17"/>
-      <c r="O76" s="17"/>
-      <c r="P76" s="17" t="s">
+      <c r="N76" s="22"/>
+      <c r="O76" s="22"/>
+      <c r="P76" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Q76" s="17"/>
-      <c r="R76" s="17"/>
-      <c r="S76" s="17" t="s">
+      <c r="Q76" s="22"/>
+      <c r="R76" s="22"/>
+      <c r="S76" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T76" s="17"/>
-      <c r="U76" s="17"/>
+      <c r="T76" s="22"/>
+      <c r="U76" s="22"/>
       <c r="W76" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="X76" s="17" t="s">
+      <c r="X76" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y76" s="17"/>
-      <c r="Z76" s="17"/>
-      <c r="AA76" s="17" t="s">
+      <c r="Y76" s="22"/>
+      <c r="Z76" s="22"/>
+      <c r="AA76" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB76" s="17"/>
-      <c r="AC76" s="17"/>
-      <c r="AD76" s="17" t="s">
+      <c r="AB76" s="22"/>
+      <c r="AC76" s="22"/>
+      <c r="AD76" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AE76" s="17"/>
-      <c r="AF76" s="17"/>
+      <c r="AE76" s="22"/>
+      <c r="AF76" s="22"/>
     </row>
     <row r="77" spans="1:32">
       <c r="A77" s="11"/>
@@ -5650,218 +5650,218 @@
       </c>
     </row>
     <row r="80" spans="1:32">
-      <c r="A80" s="18" t="s">
+      <c r="A80" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="18"/>
-      <c r="L80" s="18"/>
-      <c r="M80" s="18"/>
-      <c r="N80" s="18"/>
-      <c r="O80" s="18"/>
-      <c r="P80" s="18"/>
-      <c r="Q80" s="18"/>
-      <c r="R80" s="18"/>
-      <c r="S80" s="18"/>
-      <c r="T80" s="18"/>
-      <c r="U80" s="18"/>
-      <c r="V80" s="18"/>
-      <c r="W80" s="18"/>
-      <c r="X80" s="18"/>
-      <c r="Y80" s="18"/>
-      <c r="Z80" s="18"/>
-      <c r="AA80" s="18"/>
-      <c r="AB80" s="18"/>
-      <c r="AC80" s="18"/>
-      <c r="AD80" s="18"/>
-      <c r="AE80" s="18"/>
-      <c r="AF80" s="18"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
+      <c r="J80" s="23"/>
+      <c r="K80" s="23"/>
+      <c r="L80" s="23"/>
+      <c r="M80" s="23"/>
+      <c r="N80" s="23"/>
+      <c r="O80" s="23"/>
+      <c r="P80" s="23"/>
+      <c r="Q80" s="23"/>
+      <c r="R80" s="23"/>
+      <c r="S80" s="23"/>
+      <c r="T80" s="23"/>
+      <c r="U80" s="23"/>
+      <c r="V80" s="23"/>
+      <c r="W80" s="23"/>
+      <c r="X80" s="23"/>
+      <c r="Y80" s="23"/>
+      <c r="Z80" s="23"/>
+      <c r="AA80" s="23"/>
+      <c r="AB80" s="23"/>
+      <c r="AC80" s="23"/>
+      <c r="AD80" s="23"/>
+      <c r="AE80" s="23"/>
+      <c r="AF80" s="23"/>
     </row>
     <row r="81" spans="1:32">
-      <c r="A81" s="18"/>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="18"/>
-      <c r="K81" s="18"/>
-      <c r="L81" s="18"/>
-      <c r="M81" s="18"/>
-      <c r="N81" s="18"/>
-      <c r="O81" s="18"/>
-      <c r="P81" s="18"/>
-      <c r="Q81" s="18"/>
-      <c r="R81" s="18"/>
-      <c r="S81" s="18"/>
-      <c r="T81" s="18"/>
-      <c r="U81" s="18"/>
-      <c r="V81" s="18"/>
-      <c r="W81" s="18"/>
-      <c r="X81" s="18"/>
-      <c r="Y81" s="18"/>
-      <c r="Z81" s="18"/>
-      <c r="AA81" s="18"/>
-      <c r="AB81" s="18"/>
-      <c r="AC81" s="18"/>
-      <c r="AD81" s="18"/>
-      <c r="AE81" s="18"/>
-      <c r="AF81" s="18"/>
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="23"/>
+      <c r="H81" s="23"/>
+      <c r="I81" s="23"/>
+      <c r="J81" s="23"/>
+      <c r="K81" s="23"/>
+      <c r="L81" s="23"/>
+      <c r="M81" s="23"/>
+      <c r="N81" s="23"/>
+      <c r="O81" s="23"/>
+      <c r="P81" s="23"/>
+      <c r="Q81" s="23"/>
+      <c r="R81" s="23"/>
+      <c r="S81" s="23"/>
+      <c r="T81" s="23"/>
+      <c r="U81" s="23"/>
+      <c r="V81" s="23"/>
+      <c r="W81" s="23"/>
+      <c r="X81" s="23"/>
+      <c r="Y81" s="23"/>
+      <c r="Z81" s="23"/>
+      <c r="AA81" s="23"/>
+      <c r="AB81" s="23"/>
+      <c r="AC81" s="23"/>
+      <c r="AD81" s="23"/>
+      <c r="AE81" s="23"/>
+      <c r="AF81" s="23"/>
     </row>
     <row r="83" spans="1:32">
       <c r="A83" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="17"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="17"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="22"/>
+      <c r="J83" s="22"/>
       <c r="L83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M83" s="17" t="s">
+      <c r="M83" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N83" s="17"/>
-      <c r="O83" s="17"/>
-      <c r="P83" s="17"/>
-      <c r="Q83" s="17"/>
-      <c r="R83" s="17"/>
-      <c r="S83" s="17"/>
-      <c r="T83" s="17"/>
-      <c r="U83" s="17"/>
+      <c r="N83" s="22"/>
+      <c r="O83" s="22"/>
+      <c r="P83" s="22"/>
+      <c r="Q83" s="22"/>
+      <c r="R83" s="22"/>
+      <c r="S83" s="22"/>
+      <c r="T83" s="22"/>
+      <c r="U83" s="22"/>
       <c r="W83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X83" s="17" t="s">
+      <c r="X83" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Y83" s="17"/>
-      <c r="Z83" s="17"/>
-      <c r="AA83" s="17"/>
-      <c r="AB83" s="17"/>
-      <c r="AC83" s="17"/>
-      <c r="AD83" s="17"/>
-      <c r="AE83" s="17"/>
-      <c r="AF83" s="17"/>
+      <c r="Y83" s="22"/>
+      <c r="Z83" s="22"/>
+      <c r="AA83" s="22"/>
+      <c r="AB83" s="22"/>
+      <c r="AC83" s="22"/>
+      <c r="AD83" s="22"/>
+      <c r="AE83" s="22"/>
+      <c r="AF83" s="22"/>
     </row>
     <row r="84" spans="1:32">
       <c r="A84" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="17"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
-      <c r="J84" s="17"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
+      <c r="G84" s="22"/>
+      <c r="H84" s="22"/>
+      <c r="I84" s="22"/>
+      <c r="J84" s="22"/>
       <c r="L84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M84" s="17" t="s">
+      <c r="M84" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="N84" s="17"/>
-      <c r="O84" s="17"/>
-      <c r="P84" s="17"/>
-      <c r="Q84" s="17"/>
-      <c r="R84" s="17"/>
-      <c r="S84" s="17"/>
-      <c r="T84" s="17"/>
-      <c r="U84" s="17"/>
+      <c r="N84" s="22"/>
+      <c r="O84" s="22"/>
+      <c r="P84" s="22"/>
+      <c r="Q84" s="22"/>
+      <c r="R84" s="22"/>
+      <c r="S84" s="22"/>
+      <c r="T84" s="22"/>
+      <c r="U84" s="22"/>
       <c r="W84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X84" s="17" t="s">
+      <c r="X84" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="Y84" s="17"/>
-      <c r="Z84" s="17"/>
-      <c r="AA84" s="17"/>
-      <c r="AB84" s="17"/>
-      <c r="AC84" s="17"/>
-      <c r="AD84" s="17"/>
-      <c r="AE84" s="17"/>
-      <c r="AF84" s="17"/>
+      <c r="Y84" s="22"/>
+      <c r="Z84" s="22"/>
+      <c r="AA84" s="22"/>
+      <c r="AB84" s="22"/>
+      <c r="AC84" s="22"/>
+      <c r="AD84" s="22"/>
+      <c r="AE84" s="22"/>
+      <c r="AF84" s="22"/>
     </row>
     <row r="85" spans="1:32">
       <c r="A85" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17" t="s">
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F85" s="17"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17" t="s">
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I85" s="17"/>
-      <c r="J85" s="17"/>
+      <c r="I85" s="22"/>
+      <c r="J85" s="22"/>
       <c r="L85" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M85" s="17" t="s">
+      <c r="M85" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="N85" s="17"/>
-      <c r="O85" s="17"/>
-      <c r="P85" s="17" t="s">
+      <c r="N85" s="22"/>
+      <c r="O85" s="22"/>
+      <c r="P85" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Q85" s="17"/>
-      <c r="R85" s="17"/>
-      <c r="S85" s="17" t="s">
+      <c r="Q85" s="22"/>
+      <c r="R85" s="22"/>
+      <c r="S85" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T85" s="17"/>
-      <c r="U85" s="17"/>
+      <c r="T85" s="22"/>
+      <c r="U85" s="22"/>
       <c r="W85" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X85" s="17" t="s">
+      <c r="X85" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y85" s="17"/>
-      <c r="Z85" s="17"/>
-      <c r="AA85" s="17" t="s">
+      <c r="Y85" s="22"/>
+      <c r="Z85" s="22"/>
+      <c r="AA85" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB85" s="17"/>
-      <c r="AC85" s="17"/>
-      <c r="AD85" s="17" t="s">
+      <c r="AB85" s="22"/>
+      <c r="AC85" s="22"/>
+      <c r="AD85" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AE85" s="17"/>
-      <c r="AF85" s="17"/>
+      <c r="AE85" s="22"/>
+      <c r="AF85" s="22"/>
     </row>
     <row r="86" spans="1:32">
       <c r="B86" s="1" t="s">
@@ -6989,145 +6989,145 @@
       <c r="A99" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="17" t="s">
+      <c r="B99" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="17"/>
-      <c r="D99" s="17"/>
-      <c r="E99" s="17"/>
-      <c r="F99" s="17"/>
-      <c r="G99" s="17"/>
-      <c r="H99" s="17"/>
-      <c r="I99" s="17"/>
-      <c r="J99" s="17"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+      <c r="J99" s="22"/>
       <c r="L99" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M99" s="17" t="s">
+      <c r="M99" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="N99" s="17"/>
-      <c r="O99" s="17"/>
-      <c r="P99" s="17"/>
-      <c r="Q99" s="17"/>
-      <c r="R99" s="17"/>
-      <c r="S99" s="17"/>
-      <c r="T99" s="17"/>
-      <c r="U99" s="17"/>
+      <c r="N99" s="22"/>
+      <c r="O99" s="22"/>
+      <c r="P99" s="22"/>
+      <c r="Q99" s="22"/>
+      <c r="R99" s="22"/>
+      <c r="S99" s="22"/>
+      <c r="T99" s="22"/>
+      <c r="U99" s="22"/>
       <c r="W99" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X99" s="17" t="s">
+      <c r="X99" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="Y99" s="17"/>
-      <c r="Z99" s="17"/>
-      <c r="AA99" s="17"/>
-      <c r="AB99" s="17"/>
-      <c r="AC99" s="17"/>
-      <c r="AD99" s="17"/>
-      <c r="AE99" s="17"/>
-      <c r="AF99" s="17"/>
+      <c r="Y99" s="22"/>
+      <c r="Z99" s="22"/>
+      <c r="AA99" s="22"/>
+      <c r="AB99" s="22"/>
+      <c r="AC99" s="22"/>
+      <c r="AD99" s="22"/>
+      <c r="AE99" s="22"/>
+      <c r="AF99" s="22"/>
     </row>
     <row r="100" spans="1:32">
       <c r="A100" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="17" t="s">
+      <c r="B100" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C100" s="17"/>
-      <c r="D100" s="17"/>
-      <c r="E100" s="17"/>
-      <c r="F100" s="17"/>
-      <c r="G100" s="17"/>
-      <c r="H100" s="17"/>
-      <c r="I100" s="17"/>
-      <c r="J100" s="17"/>
+      <c r="C100" s="22"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
+      <c r="G100" s="22"/>
+      <c r="H100" s="22"/>
+      <c r="I100" s="22"/>
+      <c r="J100" s="22"/>
       <c r="L100" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M100" s="17" t="s">
+      <c r="M100" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="N100" s="17"/>
-      <c r="O100" s="17"/>
-      <c r="P100" s="17"/>
-      <c r="Q100" s="17"/>
-      <c r="R100" s="17"/>
-      <c r="S100" s="17"/>
-      <c r="T100" s="17"/>
-      <c r="U100" s="17"/>
+      <c r="N100" s="22"/>
+      <c r="O100" s="22"/>
+      <c r="P100" s="22"/>
+      <c r="Q100" s="22"/>
+      <c r="R100" s="22"/>
+      <c r="S100" s="22"/>
+      <c r="T100" s="22"/>
+      <c r="U100" s="22"/>
       <c r="W100" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X100" s="17" t="s">
+      <c r="X100" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Y100" s="17"/>
-      <c r="Z100" s="17"/>
-      <c r="AA100" s="17"/>
-      <c r="AB100" s="17"/>
-      <c r="AC100" s="17"/>
-      <c r="AD100" s="17"/>
-      <c r="AE100" s="17"/>
-      <c r="AF100" s="17"/>
+      <c r="Y100" s="22"/>
+      <c r="Z100" s="22"/>
+      <c r="AA100" s="22"/>
+      <c r="AB100" s="22"/>
+      <c r="AC100" s="22"/>
+      <c r="AD100" s="22"/>
+      <c r="AE100" s="22"/>
+      <c r="AF100" s="22"/>
     </row>
     <row r="101" spans="1:32">
       <c r="A101" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="17"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17" t="s">
+      <c r="C101" s="22"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F101" s="17"/>
-      <c r="G101" s="17"/>
-      <c r="H101" s="17" t="s">
+      <c r="F101" s="22"/>
+      <c r="G101" s="22"/>
+      <c r="H101" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I101" s="17"/>
-      <c r="J101" s="17"/>
+      <c r="I101" s="22"/>
+      <c r="J101" s="22"/>
       <c r="L101" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M101" s="19" t="s">
+      <c r="M101" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N101" s="20"/>
-      <c r="O101" s="21"/>
-      <c r="P101" s="19" t="s">
+      <c r="N101" s="18"/>
+      <c r="O101" s="19"/>
+      <c r="P101" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q101" s="20"/>
-      <c r="R101" s="21"/>
-      <c r="S101" s="17" t="s">
+      <c r="Q101" s="18"/>
+      <c r="R101" s="19"/>
+      <c r="S101" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T101" s="17"/>
-      <c r="U101" s="17"/>
+      <c r="T101" s="22"/>
+      <c r="U101" s="22"/>
       <c r="W101" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X101" s="17" t="s">
+      <c r="X101" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Y101" s="17"/>
-      <c r="Z101" s="17"/>
-      <c r="AA101" s="17" t="s">
+      <c r="Y101" s="22"/>
+      <c r="Z101" s="22"/>
+      <c r="AA101" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB101" s="17"/>
-      <c r="AC101" s="17"/>
-      <c r="AD101" s="17" t="s">
+      <c r="AB101" s="22"/>
+      <c r="AC101" s="22"/>
+      <c r="AD101" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AE101" s="17"/>
-      <c r="AF101" s="17"/>
+      <c r="AE101" s="22"/>
+      <c r="AF101" s="22"/>
     </row>
     <row r="102" spans="1:32">
       <c r="B102" s="1" t="s">
@@ -7306,52 +7306,60 @@
     </row>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="X4:AF4"/>
-    <mergeCell ref="X5:AF5"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="AD6:AF6"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="M4:U4"/>
-    <mergeCell ref="M5:U5"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="M22:U22"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B32:J32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="B50:J50"/>
-    <mergeCell ref="X23:AF23"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="M31:U31"/>
-    <mergeCell ref="A28:AF29"/>
-    <mergeCell ref="M23:U23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="M32:U32"/>
-    <mergeCell ref="X22:AF22"/>
-    <mergeCell ref="X24:Z24"/>
-    <mergeCell ref="AA24:AC24"/>
-    <mergeCell ref="AD24:AF24"/>
-    <mergeCell ref="M49:U49"/>
-    <mergeCell ref="X31:AF31"/>
-    <mergeCell ref="X32:AF32"/>
-    <mergeCell ref="X33:Z33"/>
-    <mergeCell ref="AA33:AC33"/>
-    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="X101:Z101"/>
+    <mergeCell ref="AA101:AC101"/>
+    <mergeCell ref="AD101:AF101"/>
+    <mergeCell ref="A1:AF2"/>
+    <mergeCell ref="A80:AF81"/>
+    <mergeCell ref="M101:O101"/>
+    <mergeCell ref="P101:R101"/>
+    <mergeCell ref="S101:U101"/>
+    <mergeCell ref="X83:AF83"/>
+    <mergeCell ref="X84:AF84"/>
+    <mergeCell ref="X85:Z85"/>
+    <mergeCell ref="AA85:AC85"/>
+    <mergeCell ref="AD85:AF85"/>
+    <mergeCell ref="X99:AF99"/>
+    <mergeCell ref="X100:AF100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="E101:G101"/>
+    <mergeCell ref="H101:J101"/>
+    <mergeCell ref="M83:U83"/>
+    <mergeCell ref="M84:U84"/>
+    <mergeCell ref="M85:O85"/>
+    <mergeCell ref="P85:R85"/>
+    <mergeCell ref="S85:U85"/>
+    <mergeCell ref="M99:U99"/>
+    <mergeCell ref="M100:U100"/>
+    <mergeCell ref="B84:J84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="H85:J85"/>
+    <mergeCell ref="B99:J99"/>
+    <mergeCell ref="B100:J100"/>
+    <mergeCell ref="X74:AF74"/>
+    <mergeCell ref="X75:AF75"/>
+    <mergeCell ref="X76:Z76"/>
+    <mergeCell ref="AA76:AC76"/>
+    <mergeCell ref="AD76:AF76"/>
+    <mergeCell ref="B83:J83"/>
+    <mergeCell ref="M74:U74"/>
+    <mergeCell ref="M75:U75"/>
+    <mergeCell ref="M76:O76"/>
+    <mergeCell ref="P76:R76"/>
+    <mergeCell ref="S76:U76"/>
+    <mergeCell ref="AA60:AC60"/>
+    <mergeCell ref="AD60:AF60"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="B75:J75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="H76:J76"/>
+    <mergeCell ref="M58:U58"/>
+    <mergeCell ref="M59:U59"/>
+    <mergeCell ref="M60:O60"/>
+    <mergeCell ref="P60:R60"/>
+    <mergeCell ref="S60:U60"/>
     <mergeCell ref="P33:R33"/>
     <mergeCell ref="S33:U33"/>
     <mergeCell ref="A55:AF56"/>
@@ -7376,60 +7384,52 @@
     <mergeCell ref="X58:AF58"/>
     <mergeCell ref="X59:AF59"/>
     <mergeCell ref="X60:Z60"/>
-    <mergeCell ref="AA60:AC60"/>
-    <mergeCell ref="AD60:AF60"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="B75:J75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="H76:J76"/>
-    <mergeCell ref="M58:U58"/>
-    <mergeCell ref="M59:U59"/>
-    <mergeCell ref="M60:O60"/>
-    <mergeCell ref="P60:R60"/>
-    <mergeCell ref="S60:U60"/>
-    <mergeCell ref="M100:U100"/>
-    <mergeCell ref="B84:J84"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="H85:J85"/>
-    <mergeCell ref="B99:J99"/>
-    <mergeCell ref="B100:J100"/>
-    <mergeCell ref="X74:AF74"/>
-    <mergeCell ref="X75:AF75"/>
-    <mergeCell ref="X76:Z76"/>
-    <mergeCell ref="AA76:AC76"/>
-    <mergeCell ref="AD76:AF76"/>
-    <mergeCell ref="B83:J83"/>
-    <mergeCell ref="M74:U74"/>
-    <mergeCell ref="M75:U75"/>
-    <mergeCell ref="M76:O76"/>
-    <mergeCell ref="P76:R76"/>
-    <mergeCell ref="S76:U76"/>
-    <mergeCell ref="X101:Z101"/>
-    <mergeCell ref="AA101:AC101"/>
-    <mergeCell ref="AD101:AF101"/>
-    <mergeCell ref="A1:AF2"/>
-    <mergeCell ref="A80:AF81"/>
-    <mergeCell ref="M101:O101"/>
-    <mergeCell ref="P101:R101"/>
-    <mergeCell ref="S101:U101"/>
-    <mergeCell ref="X83:AF83"/>
-    <mergeCell ref="X84:AF84"/>
-    <mergeCell ref="X85:Z85"/>
-    <mergeCell ref="AA85:AC85"/>
-    <mergeCell ref="AD85:AF85"/>
-    <mergeCell ref="X99:AF99"/>
-    <mergeCell ref="X100:AF100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="E101:G101"/>
-    <mergeCell ref="H101:J101"/>
-    <mergeCell ref="M83:U83"/>
-    <mergeCell ref="M84:U84"/>
-    <mergeCell ref="M85:O85"/>
-    <mergeCell ref="P85:R85"/>
-    <mergeCell ref="S85:U85"/>
-    <mergeCell ref="M99:U99"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="B50:J50"/>
+    <mergeCell ref="X23:AF23"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="M31:U31"/>
+    <mergeCell ref="A28:AF29"/>
+    <mergeCell ref="M23:U23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="M32:U32"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="AA24:AC24"/>
+    <mergeCell ref="AD24:AF24"/>
+    <mergeCell ref="M49:U49"/>
+    <mergeCell ref="X31:AF31"/>
+    <mergeCell ref="X32:AF32"/>
+    <mergeCell ref="X33:Z33"/>
+    <mergeCell ref="AA33:AC33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="X4:AF4"/>
+    <mergeCell ref="X5:AF5"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="M4:U4"/>
+    <mergeCell ref="M5:U5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="M22:U22"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="X22:AF22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dodano: ekperyment 2, podsumoanie i wnioski, geneza i opis rodziałów
</commit_message>
<xml_diff>
--- a/doc/Wyniki_end.xlsx
+++ b/doc/Wyniki_end.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="39">
   <si>
     <t>Rozmiar grafu:</t>
   </si>
@@ -116,12 +116,30 @@
   <si>
     <t>Mapa 2</t>
   </si>
+  <si>
+    <t>50z50</t>
+  </si>
+  <si>
+    <t>lab</t>
+  </si>
+  <si>
+    <t>long path</t>
+  </si>
+  <si>
+    <t>slepa</t>
+  </si>
+  <si>
+    <t>prosta</t>
+  </si>
+  <si>
+    <t>Map 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +158,25 @@
     </font>
     <font>
       <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -316,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -344,6 +381,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -355,12 +398,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -662,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF103"/>
+  <dimension ref="A1:AF121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4:AF18"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -674,218 +719,218 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
     </row>
     <row r="2" spans="1:32">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="L4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
       <c r="W4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X4" s="17" t="s">
+      <c r="X4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="19"/>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+      <c r="AC4" s="20"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="21"/>
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
       <c r="L5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="22"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
       <c r="W5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X5" s="17" t="s">
+      <c r="X5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="18"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="19"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="21"/>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="22"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="22" t="s">
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22" t="s">
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T6" s="22"/>
-      <c r="U6" s="22"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
       <c r="W6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X6" s="17" t="s">
+      <c r="X6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="17" t="s">
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="17" t="s">
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="19"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="21"/>
     </row>
     <row r="7" spans="1:32">
       <c r="B7" s="1" t="s">
@@ -2015,145 +2060,145 @@
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="21"/>
       <c r="L22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="17" t="s">
+      <c r="M22" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="19"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="21"/>
       <c r="W22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X22" s="17" t="s">
+      <c r="X22" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
-      <c r="AB22" s="18"/>
-      <c r="AC22" s="18"/>
-      <c r="AD22" s="18"/>
-      <c r="AE22" s="18"/>
-      <c r="AF22" s="19"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="20"/>
+      <c r="AD22" s="20"/>
+      <c r="AE22" s="20"/>
+      <c r="AF22" s="21"/>
     </row>
     <row r="23" spans="1:32">
       <c r="A23" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="21"/>
       <c r="L23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M23" s="17" t="s">
+      <c r="M23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="19"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="21"/>
       <c r="W23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X23" s="17" t="s">
+      <c r="X23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="Y23" s="18"/>
-      <c r="Z23" s="18"/>
-      <c r="AA23" s="18"/>
-      <c r="AB23" s="18"/>
-      <c r="AC23" s="18"/>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="18"/>
-      <c r="AF23" s="19"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20"/>
+      <c r="AD23" s="20"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="21"/>
     </row>
     <row r="24" spans="1:32">
       <c r="A24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="17" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="17" t="s">
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="21"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="23"/>
       <c r="L24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M24" s="17" t="s">
+      <c r="M24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N24" s="18"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="17" t="s">
+      <c r="N24" s="20"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="19"/>
-      <c r="S24" s="22" t="s">
+      <c r="Q24" s="20"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T24" s="22"/>
-      <c r="U24" s="22"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
       <c r="W24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X24" s="17" t="s">
+      <c r="X24" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="Y24" s="18"/>
-      <c r="Z24" s="19"/>
-      <c r="AA24" s="17" t="s">
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AB24" s="18"/>
-      <c r="AC24" s="19"/>
-      <c r="AD24" s="17" t="s">
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="21"/>
+      <c r="AD24" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AE24" s="18"/>
-      <c r="AF24" s="19"/>
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="21"/>
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="9"/>
@@ -2334,218 +2379,218 @@
       </c>
     </row>
     <row r="28" spans="1:32">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="23"/>
-      <c r="X28" s="23"/>
-      <c r="Y28" s="23"/>
-      <c r="Z28" s="23"/>
-      <c r="AA28" s="23"/>
-      <c r="AB28" s="23"/>
-      <c r="AC28" s="23"/>
-      <c r="AD28" s="23"/>
-      <c r="AE28" s="23"/>
-      <c r="AF28" s="23"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18"/>
+      <c r="V28" s="18"/>
+      <c r="W28" s="18"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+      <c r="AB28" s="18"/>
+      <c r="AC28" s="18"/>
+      <c r="AD28" s="18"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="18"/>
     </row>
     <row r="29" spans="1:32">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="23"/>
-      <c r="Z29" s="23"/>
-      <c r="AA29" s="23"/>
-      <c r="AB29" s="23"/>
-      <c r="AC29" s="23"/>
-      <c r="AD29" s="23"/>
-      <c r="AE29" s="23"/>
-      <c r="AF29" s="23"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+      <c r="W29" s="18"/>
+      <c r="X29" s="18"/>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="18"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="18"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="18"/>
     </row>
     <row r="31" spans="1:32">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
       <c r="L31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M31" s="22" t="s">
+      <c r="M31" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="22"/>
-      <c r="S31" s="22"/>
-      <c r="T31" s="22"/>
-      <c r="U31" s="22"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
       <c r="W31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X31" s="22" t="s">
+      <c r="X31" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y31" s="22"/>
-      <c r="Z31" s="22"/>
-      <c r="AA31" s="22"/>
-      <c r="AB31" s="22"/>
-      <c r="AC31" s="22"/>
-      <c r="AD31" s="22"/>
-      <c r="AE31" s="22"/>
-      <c r="AF31" s="22"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="17"/>
+      <c r="AD31" s="17"/>
+      <c r="AE31" s="17"/>
+      <c r="AF31" s="17"/>
     </row>
     <row r="32" spans="1:32">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
       <c r="L32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M32" s="22" t="s">
+      <c r="M32" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="22"/>
-      <c r="S32" s="22"/>
-      <c r="T32" s="22"/>
-      <c r="U32" s="22"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
       <c r="W32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X32" s="22" t="s">
+      <c r="X32" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Y32" s="22"/>
-      <c r="Z32" s="22"/>
-      <c r="AA32" s="22"/>
-      <c r="AB32" s="22"/>
-      <c r="AC32" s="22"/>
-      <c r="AD32" s="22"/>
-      <c r="AE32" s="22"/>
-      <c r="AF32" s="22"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17"/>
+      <c r="AD32" s="17"/>
+      <c r="AE32" s="17"/>
+      <c r="AF32" s="17"/>
     </row>
     <row r="33" spans="1:32">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22" t="s">
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22" t="s">
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
       <c r="L33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="M33" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22" t="s">
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q33" s="22"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="22" t="s">
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T33" s="22"/>
-      <c r="U33" s="22"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
       <c r="W33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X33" s="22" t="s">
+      <c r="X33" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y33" s="22"/>
-      <c r="Z33" s="22"/>
-      <c r="AA33" s="22" t="s">
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB33" s="22"/>
-      <c r="AC33" s="22"/>
-      <c r="AD33" s="22" t="s">
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE33" s="22"/>
-      <c r="AF33" s="22"/>
+      <c r="AE33" s="17"/>
+      <c r="AF33" s="17"/>
     </row>
     <row r="34" spans="1:32">
       <c r="B34" s="1" t="s">
@@ -3674,145 +3719,145 @@
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
       <c r="L49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M49" s="22" t="s">
+      <c r="M49" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N49" s="22"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="22"/>
-      <c r="Q49" s="22"/>
-      <c r="R49" s="22"/>
-      <c r="S49" s="22"/>
-      <c r="T49" s="22"/>
-      <c r="U49" s="22"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
       <c r="W49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X49" s="22" t="s">
+      <c r="X49" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y49" s="22"/>
-      <c r="Z49" s="22"/>
-      <c r="AA49" s="22"/>
-      <c r="AB49" s="22"/>
-      <c r="AC49" s="22"/>
-      <c r="AD49" s="22"/>
-      <c r="AE49" s="22"/>
-      <c r="AF49" s="22"/>
+      <c r="Y49" s="17"/>
+      <c r="Z49" s="17"/>
+      <c r="AA49" s="17"/>
+      <c r="AB49" s="17"/>
+      <c r="AC49" s="17"/>
+      <c r="AD49" s="17"/>
+      <c r="AE49" s="17"/>
+      <c r="AF49" s="17"/>
     </row>
     <row r="50" spans="1:32">
       <c r="A50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-      <c r="J50" s="22"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
       <c r="L50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M50" s="22" t="s">
+      <c r="M50" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N50" s="22"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="22"/>
-      <c r="Q50" s="22"/>
-      <c r="R50" s="22"/>
-      <c r="S50" s="22"/>
-      <c r="T50" s="22"/>
-      <c r="U50" s="22"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="17"/>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17"/>
       <c r="W50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X50" s="22" t="s">
+      <c r="X50" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Y50" s="22"/>
-      <c r="Z50" s="22"/>
-      <c r="AA50" s="22"/>
-      <c r="AB50" s="22"/>
-      <c r="AC50" s="22"/>
-      <c r="AD50" s="22"/>
-      <c r="AE50" s="22"/>
-      <c r="AF50" s="22"/>
+      <c r="Y50" s="17"/>
+      <c r="Z50" s="17"/>
+      <c r="AA50" s="17"/>
+      <c r="AB50" s="17"/>
+      <c r="AC50" s="17"/>
+      <c r="AD50" s="17"/>
+      <c r="AE50" s="17"/>
+      <c r="AF50" s="17"/>
     </row>
     <row r="51" spans="1:32">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22" t="s">
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22" t="s">
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
       <c r="L51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M51" s="22" t="s">
+      <c r="M51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22" t="s">
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q51" s="22"/>
-      <c r="R51" s="22"/>
-      <c r="S51" s="22" t="s">
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T51" s="22"/>
-      <c r="U51" s="22"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17"/>
       <c r="W51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X51" s="22" t="s">
+      <c r="X51" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y51" s="22"/>
-      <c r="Z51" s="22"/>
-      <c r="AA51" s="22" t="s">
+      <c r="Y51" s="17"/>
+      <c r="Z51" s="17"/>
+      <c r="AA51" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB51" s="22"/>
-      <c r="AC51" s="22"/>
-      <c r="AD51" s="22" t="s">
+      <c r="AB51" s="17"/>
+      <c r="AC51" s="17"/>
+      <c r="AD51" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE51" s="22"/>
-      <c r="AF51" s="22"/>
+      <c r="AE51" s="17"/>
+      <c r="AF51" s="17"/>
     </row>
     <row r="52" spans="1:32">
       <c r="A52" s="11"/>
@@ -3993,218 +4038,218 @@
       </c>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="23"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="23"/>
-      <c r="I55" s="23"/>
-      <c r="J55" s="23"/>
-      <c r="K55" s="23"/>
-      <c r="L55" s="23"/>
-      <c r="M55" s="23"/>
-      <c r="N55" s="23"/>
-      <c r="O55" s="23"/>
-      <c r="P55" s="23"/>
-      <c r="Q55" s="23"/>
-      <c r="R55" s="23"/>
-      <c r="S55" s="23"/>
-      <c r="T55" s="23"/>
-      <c r="U55" s="23"/>
-      <c r="V55" s="23"/>
-      <c r="W55" s="23"/>
-      <c r="X55" s="23"/>
-      <c r="Y55" s="23"/>
-      <c r="Z55" s="23"/>
-      <c r="AA55" s="23"/>
-      <c r="AB55" s="23"/>
-      <c r="AC55" s="23"/>
-      <c r="AD55" s="23"/>
-      <c r="AE55" s="23"/>
-      <c r="AF55" s="23"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="18"/>
+      <c r="U55" s="18"/>
+      <c r="V55" s="18"/>
+      <c r="W55" s="18"/>
+      <c r="X55" s="18"/>
+      <c r="Y55" s="18"/>
+      <c r="Z55" s="18"/>
+      <c r="AA55" s="18"/>
+      <c r="AB55" s="18"/>
+      <c r="AC55" s="18"/>
+      <c r="AD55" s="18"/>
+      <c r="AE55" s="18"/>
+      <c r="AF55" s="18"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="23"/>
-      <c r="B56" s="23"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="23"/>
-      <c r="I56" s="23"/>
-      <c r="J56" s="23"/>
-      <c r="K56" s="23"/>
-      <c r="L56" s="23"/>
-      <c r="M56" s="23"/>
-      <c r="N56" s="23"/>
-      <c r="O56" s="23"/>
-      <c r="P56" s="23"/>
-      <c r="Q56" s="23"/>
-      <c r="R56" s="23"/>
-      <c r="S56" s="23"/>
-      <c r="T56" s="23"/>
-      <c r="U56" s="23"/>
-      <c r="V56" s="23"/>
-      <c r="W56" s="23"/>
-      <c r="X56" s="23"/>
-      <c r="Y56" s="23"/>
-      <c r="Z56" s="23"/>
-      <c r="AA56" s="23"/>
-      <c r="AB56" s="23"/>
-      <c r="AC56" s="23"/>
-      <c r="AD56" s="23"/>
-      <c r="AE56" s="23"/>
-      <c r="AF56" s="23"/>
+      <c r="A56" s="18"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="18"/>
+      <c r="U56" s="18"/>
+      <c r="V56" s="18"/>
+      <c r="W56" s="18"/>
+      <c r="X56" s="18"/>
+      <c r="Y56" s="18"/>
+      <c r="Z56" s="18"/>
+      <c r="AA56" s="18"/>
+      <c r="AB56" s="18"/>
+      <c r="AC56" s="18"/>
+      <c r="AD56" s="18"/>
+      <c r="AE56" s="18"/>
+      <c r="AF56" s="18"/>
     </row>
     <row r="58" spans="1:32">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
       <c r="L58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M58" s="22" t="s">
+      <c r="M58" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N58" s="22"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
-      <c r="S58" s="22"/>
-      <c r="T58" s="22"/>
-      <c r="U58" s="22"/>
+      <c r="N58" s="17"/>
+      <c r="O58" s="17"/>
+      <c r="P58" s="17"/>
+      <c r="Q58" s="17"/>
+      <c r="R58" s="17"/>
+      <c r="S58" s="17"/>
+      <c r="T58" s="17"/>
+      <c r="U58" s="17"/>
       <c r="W58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X58" s="22" t="s">
+      <c r="X58" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y58" s="22"/>
-      <c r="Z58" s="22"/>
-      <c r="AA58" s="22"/>
-      <c r="AB58" s="22"/>
-      <c r="AC58" s="22"/>
-      <c r="AD58" s="22"/>
-      <c r="AE58" s="22"/>
-      <c r="AF58" s="22"/>
+      <c r="Y58" s="17"/>
+      <c r="Z58" s="17"/>
+      <c r="AA58" s="17"/>
+      <c r="AB58" s="17"/>
+      <c r="AC58" s="17"/>
+      <c r="AD58" s="17"/>
+      <c r="AE58" s="17"/>
+      <c r="AF58" s="17"/>
     </row>
     <row r="59" spans="1:32">
       <c r="A59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
       <c r="L59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M59" s="22" t="s">
+      <c r="M59" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N59" s="22"/>
-      <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22"/>
-      <c r="S59" s="22"/>
-      <c r="T59" s="22"/>
-      <c r="U59" s="22"/>
+      <c r="N59" s="17"/>
+      <c r="O59" s="17"/>
+      <c r="P59" s="17"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="17"/>
+      <c r="S59" s="17"/>
+      <c r="T59" s="17"/>
+      <c r="U59" s="17"/>
       <c r="W59" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X59" s="22" t="s">
+      <c r="X59" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Y59" s="22"/>
-      <c r="Z59" s="22"/>
-      <c r="AA59" s="22"/>
-      <c r="AB59" s="22"/>
-      <c r="AC59" s="22"/>
-      <c r="AD59" s="22"/>
-      <c r="AE59" s="22"/>
-      <c r="AF59" s="22"/>
+      <c r="Y59" s="17"/>
+      <c r="Z59" s="17"/>
+      <c r="AA59" s="17"/>
+      <c r="AB59" s="17"/>
+      <c r="AC59" s="17"/>
+      <c r="AD59" s="17"/>
+      <c r="AE59" s="17"/>
+      <c r="AF59" s="17"/>
     </row>
     <row r="60" spans="1:32">
       <c r="A60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="17" t="s">
+      <c r="C60" s="20"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="18"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="22" t="s">
+      <c r="F60" s="20"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
       <c r="L60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M60" s="17" t="s">
+      <c r="M60" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N60" s="18"/>
-      <c r="O60" s="19"/>
-      <c r="P60" s="17" t="s">
+      <c r="N60" s="20"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="19"/>
-      <c r="S60" s="22" t="s">
+      <c r="Q60" s="20"/>
+      <c r="R60" s="21"/>
+      <c r="S60" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T60" s="22"/>
-      <c r="U60" s="22"/>
+      <c r="T60" s="17"/>
+      <c r="U60" s="17"/>
       <c r="W60" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X60" s="22" t="s">
+      <c r="X60" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y60" s="22"/>
-      <c r="Z60" s="22"/>
-      <c r="AA60" s="22" t="s">
+      <c r="Y60" s="17"/>
+      <c r="Z60" s="17"/>
+      <c r="AA60" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB60" s="22"/>
-      <c r="AC60" s="22"/>
-      <c r="AD60" s="22" t="s">
+      <c r="AB60" s="17"/>
+      <c r="AC60" s="17"/>
+      <c r="AD60" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE60" s="22"/>
-      <c r="AF60" s="22"/>
+      <c r="AE60" s="17"/>
+      <c r="AF60" s="17"/>
     </row>
     <row r="61" spans="1:32">
       <c r="A61" s="11"/>
@@ -5333,145 +5378,145 @@
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="22"/>
-      <c r="G74" s="22"/>
-      <c r="H74" s="22"/>
-      <c r="I74" s="22"/>
-      <c r="J74" s="22"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+      <c r="J74" s="17"/>
       <c r="L74" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M74" s="22" t="s">
+      <c r="M74" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N74" s="22"/>
-      <c r="O74" s="22"/>
-      <c r="P74" s="22"/>
-      <c r="Q74" s="22"/>
-      <c r="R74" s="22"/>
-      <c r="S74" s="22"/>
-      <c r="T74" s="22"/>
-      <c r="U74" s="22"/>
+      <c r="N74" s="17"/>
+      <c r="O74" s="17"/>
+      <c r="P74" s="17"/>
+      <c r="Q74" s="17"/>
+      <c r="R74" s="17"/>
+      <c r="S74" s="17"/>
+      <c r="T74" s="17"/>
+      <c r="U74" s="17"/>
       <c r="W74" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="X74" s="22" t="s">
+      <c r="X74" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y74" s="22"/>
-      <c r="Z74" s="22"/>
-      <c r="AA74" s="22"/>
-      <c r="AB74" s="22"/>
-      <c r="AC74" s="22"/>
-      <c r="AD74" s="22"/>
-      <c r="AE74" s="22"/>
-      <c r="AF74" s="22"/>
+      <c r="Y74" s="17"/>
+      <c r="Z74" s="17"/>
+      <c r="AA74" s="17"/>
+      <c r="AB74" s="17"/>
+      <c r="AC74" s="17"/>
+      <c r="AD74" s="17"/>
+      <c r="AE74" s="17"/>
+      <c r="AF74" s="17"/>
     </row>
     <row r="75" spans="1:32">
       <c r="A75" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-      <c r="G75" s="22"/>
-      <c r="H75" s="22"/>
-      <c r="I75" s="22"/>
-      <c r="J75" s="22"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
       <c r="L75" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M75" s="22" t="s">
+      <c r="M75" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N75" s="22"/>
-      <c r="O75" s="22"/>
-      <c r="P75" s="22"/>
-      <c r="Q75" s="22"/>
-      <c r="R75" s="22"/>
-      <c r="S75" s="22"/>
-      <c r="T75" s="22"/>
-      <c r="U75" s="22"/>
+      <c r="N75" s="17"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="17"/>
+      <c r="Q75" s="17"/>
+      <c r="R75" s="17"/>
+      <c r="S75" s="17"/>
+      <c r="T75" s="17"/>
+      <c r="U75" s="17"/>
       <c r="W75" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="X75" s="22" t="s">
+      <c r="X75" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Y75" s="22"/>
-      <c r="Z75" s="22"/>
-      <c r="AA75" s="22"/>
-      <c r="AB75" s="22"/>
-      <c r="AC75" s="22"/>
-      <c r="AD75" s="22"/>
-      <c r="AE75" s="22"/>
-      <c r="AF75" s="22"/>
+      <c r="Y75" s="17"/>
+      <c r="Z75" s="17"/>
+      <c r="AA75" s="17"/>
+      <c r="AB75" s="17"/>
+      <c r="AC75" s="17"/>
+      <c r="AD75" s="17"/>
+      <c r="AE75" s="17"/>
+      <c r="AF75" s="17"/>
     </row>
     <row r="76" spans="1:32">
       <c r="A76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C76" s="18"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="17" t="s">
+      <c r="C76" s="20"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F76" s="18"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="22" t="s">
+      <c r="F76" s="20"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I76" s="22"/>
-      <c r="J76" s="22"/>
+      <c r="I76" s="17"/>
+      <c r="J76" s="17"/>
       <c r="L76" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M76" s="22" t="s">
+      <c r="M76" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N76" s="22"/>
-      <c r="O76" s="22"/>
-      <c r="P76" s="22" t="s">
+      <c r="N76" s="17"/>
+      <c r="O76" s="17"/>
+      <c r="P76" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q76" s="22"/>
-      <c r="R76" s="22"/>
-      <c r="S76" s="22" t="s">
+      <c r="Q76" s="17"/>
+      <c r="R76" s="17"/>
+      <c r="S76" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T76" s="22"/>
-      <c r="U76" s="22"/>
+      <c r="T76" s="17"/>
+      <c r="U76" s="17"/>
       <c r="W76" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="X76" s="22" t="s">
+      <c r="X76" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y76" s="22"/>
-      <c r="Z76" s="22"/>
-      <c r="AA76" s="22" t="s">
+      <c r="Y76" s="17"/>
+      <c r="Z76" s="17"/>
+      <c r="AA76" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB76" s="22"/>
-      <c r="AC76" s="22"/>
-      <c r="AD76" s="22" t="s">
+      <c r="AB76" s="17"/>
+      <c r="AC76" s="17"/>
+      <c r="AD76" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE76" s="22"/>
-      <c r="AF76" s="22"/>
+      <c r="AE76" s="17"/>
+      <c r="AF76" s="17"/>
     </row>
     <row r="77" spans="1:32">
       <c r="A77" s="11"/>
@@ -5650,218 +5695,218 @@
       </c>
     </row>
     <row r="80" spans="1:32">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B80" s="23"/>
-      <c r="C80" s="23"/>
-      <c r="D80" s="23"/>
-      <c r="E80" s="23"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="23"/>
-      <c r="H80" s="23"/>
-      <c r="I80" s="23"/>
-      <c r="J80" s="23"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="23"/>
-      <c r="M80" s="23"/>
-      <c r="N80" s="23"/>
-      <c r="O80" s="23"/>
-      <c r="P80" s="23"/>
-      <c r="Q80" s="23"/>
-      <c r="R80" s="23"/>
-      <c r="S80" s="23"/>
-      <c r="T80" s="23"/>
-      <c r="U80" s="23"/>
-      <c r="V80" s="23"/>
-      <c r="W80" s="23"/>
-      <c r="X80" s="23"/>
-      <c r="Y80" s="23"/>
-      <c r="Z80" s="23"/>
-      <c r="AA80" s="23"/>
-      <c r="AB80" s="23"/>
-      <c r="AC80" s="23"/>
-      <c r="AD80" s="23"/>
-      <c r="AE80" s="23"/>
-      <c r="AF80" s="23"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="18"/>
+      <c r="M80" s="18"/>
+      <c r="N80" s="18"/>
+      <c r="O80" s="18"/>
+      <c r="P80" s="18"/>
+      <c r="Q80" s="18"/>
+      <c r="R80" s="18"/>
+      <c r="S80" s="18"/>
+      <c r="T80" s="18"/>
+      <c r="U80" s="18"/>
+      <c r="V80" s="18"/>
+      <c r="W80" s="18"/>
+      <c r="X80" s="18"/>
+      <c r="Y80" s="18"/>
+      <c r="Z80" s="18"/>
+      <c r="AA80" s="18"/>
+      <c r="AB80" s="18"/>
+      <c r="AC80" s="18"/>
+      <c r="AD80" s="18"/>
+      <c r="AE80" s="18"/>
+      <c r="AF80" s="18"/>
     </row>
     <row r="81" spans="1:32">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
-      <c r="H81" s="23"/>
-      <c r="I81" s="23"/>
-      <c r="J81" s="23"/>
-      <c r="K81" s="23"/>
-      <c r="L81" s="23"/>
-      <c r="M81" s="23"/>
-      <c r="N81" s="23"/>
-      <c r="O81" s="23"/>
-      <c r="P81" s="23"/>
-      <c r="Q81" s="23"/>
-      <c r="R81" s="23"/>
-      <c r="S81" s="23"/>
-      <c r="T81" s="23"/>
-      <c r="U81" s="23"/>
-      <c r="V81" s="23"/>
-      <c r="W81" s="23"/>
-      <c r="X81" s="23"/>
-      <c r="Y81" s="23"/>
-      <c r="Z81" s="23"/>
-      <c r="AA81" s="23"/>
-      <c r="AB81" s="23"/>
-      <c r="AC81" s="23"/>
-      <c r="AD81" s="23"/>
-      <c r="AE81" s="23"/>
-      <c r="AF81" s="23"/>
+      <c r="A81" s="18"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="18"/>
+      <c r="R81" s="18"/>
+      <c r="S81" s="18"/>
+      <c r="T81" s="18"/>
+      <c r="U81" s="18"/>
+      <c r="V81" s="18"/>
+      <c r="W81" s="18"/>
+      <c r="X81" s="18"/>
+      <c r="Y81" s="18"/>
+      <c r="Z81" s="18"/>
+      <c r="AA81" s="18"/>
+      <c r="AB81" s="18"/>
+      <c r="AC81" s="18"/>
+      <c r="AD81" s="18"/>
+      <c r="AE81" s="18"/>
+      <c r="AF81" s="18"/>
     </row>
     <row r="83" spans="1:32">
       <c r="A83" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B83" s="22" t="s">
+      <c r="B83" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22"/>
-      <c r="E83" s="22"/>
-      <c r="F83" s="22"/>
-      <c r="G83" s="22"/>
-      <c r="H83" s="22"/>
-      <c r="I83" s="22"/>
-      <c r="J83" s="22"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+      <c r="J83" s="17"/>
       <c r="L83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M83" s="22" t="s">
+      <c r="M83" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N83" s="22"/>
-      <c r="O83" s="22"/>
-      <c r="P83" s="22"/>
-      <c r="Q83" s="22"/>
-      <c r="R83" s="22"/>
-      <c r="S83" s="22"/>
-      <c r="T83" s="22"/>
-      <c r="U83" s="22"/>
+      <c r="N83" s="17"/>
+      <c r="O83" s="17"/>
+      <c r="P83" s="17"/>
+      <c r="Q83" s="17"/>
+      <c r="R83" s="17"/>
+      <c r="S83" s="17"/>
+      <c r="T83" s="17"/>
+      <c r="U83" s="17"/>
       <c r="W83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X83" s="22" t="s">
+      <c r="X83" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y83" s="22"/>
-      <c r="Z83" s="22"/>
-      <c r="AA83" s="22"/>
-      <c r="AB83" s="22"/>
-      <c r="AC83" s="22"/>
-      <c r="AD83" s="22"/>
-      <c r="AE83" s="22"/>
-      <c r="AF83" s="22"/>
+      <c r="Y83" s="17"/>
+      <c r="Z83" s="17"/>
+      <c r="AA83" s="17"/>
+      <c r="AB83" s="17"/>
+      <c r="AC83" s="17"/>
+      <c r="AD83" s="17"/>
+      <c r="AE83" s="17"/>
+      <c r="AF83" s="17"/>
     </row>
     <row r="84" spans="1:32">
       <c r="A84" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B84" s="22" t="s">
+      <c r="B84" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C84" s="22"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="22"/>
-      <c r="G84" s="22"/>
-      <c r="H84" s="22"/>
-      <c r="I84" s="22"/>
-      <c r="J84" s="22"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="17"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+      <c r="J84" s="17"/>
       <c r="L84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M84" s="22" t="s">
+      <c r="M84" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="N84" s="22"/>
-      <c r="O84" s="22"/>
-      <c r="P84" s="22"/>
-      <c r="Q84" s="22"/>
-      <c r="R84" s="22"/>
-      <c r="S84" s="22"/>
-      <c r="T84" s="22"/>
-      <c r="U84" s="22"/>
+      <c r="N84" s="17"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="17"/>
+      <c r="Q84" s="17"/>
+      <c r="R84" s="17"/>
+      <c r="S84" s="17"/>
+      <c r="T84" s="17"/>
+      <c r="U84" s="17"/>
       <c r="W84" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X84" s="22" t="s">
+      <c r="X84" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="Y84" s="22"/>
-      <c r="Z84" s="22"/>
-      <c r="AA84" s="22"/>
-      <c r="AB84" s="22"/>
-      <c r="AC84" s="22"/>
-      <c r="AD84" s="22"/>
-      <c r="AE84" s="22"/>
-      <c r="AF84" s="22"/>
+      <c r="Y84" s="17"/>
+      <c r="Z84" s="17"/>
+      <c r="AA84" s="17"/>
+      <c r="AB84" s="17"/>
+      <c r="AC84" s="17"/>
+      <c r="AD84" s="17"/>
+      <c r="AE84" s="17"/>
+      <c r="AF84" s="17"/>
     </row>
     <row r="85" spans="1:32">
       <c r="A85" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="22" t="s">
+      <c r="C85" s="17"/>
+      <c r="D85" s="17"/>
+      <c r="E85" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F85" s="22"/>
-      <c r="G85" s="22"/>
-      <c r="H85" s="22" t="s">
+      <c r="F85" s="17"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I85" s="22"/>
-      <c r="J85" s="22"/>
+      <c r="I85" s="17"/>
+      <c r="J85" s="17"/>
       <c r="L85" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M85" s="22" t="s">
+      <c r="M85" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="N85" s="22"/>
-      <c r="O85" s="22"/>
-      <c r="P85" s="22" t="s">
+      <c r="N85" s="17"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="Q85" s="22"/>
-      <c r="R85" s="22"/>
-      <c r="S85" s="22" t="s">
+      <c r="Q85" s="17"/>
+      <c r="R85" s="17"/>
+      <c r="S85" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T85" s="22"/>
-      <c r="U85" s="22"/>
+      <c r="T85" s="17"/>
+      <c r="U85" s="17"/>
       <c r="W85" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X85" s="22" t="s">
+      <c r="X85" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y85" s="22"/>
-      <c r="Z85" s="22"/>
-      <c r="AA85" s="22" t="s">
+      <c r="Y85" s="17"/>
+      <c r="Z85" s="17"/>
+      <c r="AA85" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB85" s="22"/>
-      <c r="AC85" s="22"/>
-      <c r="AD85" s="22" t="s">
+      <c r="AB85" s="17"/>
+      <c r="AC85" s="17"/>
+      <c r="AD85" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE85" s="22"/>
-      <c r="AF85" s="22"/>
+      <c r="AE85" s="17"/>
+      <c r="AF85" s="17"/>
     </row>
     <row r="86" spans="1:32">
       <c r="B86" s="1" t="s">
@@ -6989,145 +7034,145 @@
       <c r="A99" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C99" s="22"/>
-      <c r="D99" s="22"/>
-      <c r="E99" s="22"/>
-      <c r="F99" s="22"/>
-      <c r="G99" s="22"/>
-      <c r="H99" s="22"/>
-      <c r="I99" s="22"/>
-      <c r="J99" s="22"/>
+      <c r="C99" s="17"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="17"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
+      <c r="J99" s="17"/>
       <c r="L99" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M99" s="22" t="s">
+      <c r="M99" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="N99" s="22"/>
-      <c r="O99" s="22"/>
-      <c r="P99" s="22"/>
-      <c r="Q99" s="22"/>
-      <c r="R99" s="22"/>
-      <c r="S99" s="22"/>
-      <c r="T99" s="22"/>
-      <c r="U99" s="22"/>
+      <c r="N99" s="17"/>
+      <c r="O99" s="17"/>
+      <c r="P99" s="17"/>
+      <c r="Q99" s="17"/>
+      <c r="R99" s="17"/>
+      <c r="S99" s="17"/>
+      <c r="T99" s="17"/>
+      <c r="U99" s="17"/>
       <c r="W99" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X99" s="22" t="s">
+      <c r="X99" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="Y99" s="22"/>
-      <c r="Z99" s="22"/>
-      <c r="AA99" s="22"/>
-      <c r="AB99" s="22"/>
-      <c r="AC99" s="22"/>
-      <c r="AD99" s="22"/>
-      <c r="AE99" s="22"/>
-      <c r="AF99" s="22"/>
+      <c r="Y99" s="17"/>
+      <c r="Z99" s="17"/>
+      <c r="AA99" s="17"/>
+      <c r="AB99" s="17"/>
+      <c r="AC99" s="17"/>
+      <c r="AD99" s="17"/>
+      <c r="AE99" s="17"/>
+      <c r="AF99" s="17"/>
     </row>
     <row r="100" spans="1:32">
       <c r="A100" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="22" t="s">
+      <c r="B100" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C100" s="22"/>
-      <c r="D100" s="22"/>
-      <c r="E100" s="22"/>
-      <c r="F100" s="22"/>
-      <c r="G100" s="22"/>
-      <c r="H100" s="22"/>
-      <c r="I100" s="22"/>
-      <c r="J100" s="22"/>
+      <c r="C100" s="17"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
+      <c r="J100" s="17"/>
       <c r="L100" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M100" s="22" t="s">
+      <c r="M100" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="N100" s="22"/>
-      <c r="O100" s="22"/>
-      <c r="P100" s="22"/>
-      <c r="Q100" s="22"/>
-      <c r="R100" s="22"/>
-      <c r="S100" s="22"/>
-      <c r="T100" s="22"/>
-      <c r="U100" s="22"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="17"/>
+      <c r="Q100" s="17"/>
+      <c r="R100" s="17"/>
+      <c r="S100" s="17"/>
+      <c r="T100" s="17"/>
+      <c r="U100" s="17"/>
       <c r="W100" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X100" s="22" t="s">
+      <c r="X100" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Y100" s="22"/>
-      <c r="Z100" s="22"/>
-      <c r="AA100" s="22"/>
-      <c r="AB100" s="22"/>
-      <c r="AC100" s="22"/>
-      <c r="AD100" s="22"/>
-      <c r="AE100" s="22"/>
-      <c r="AF100" s="22"/>
+      <c r="Y100" s="17"/>
+      <c r="Z100" s="17"/>
+      <c r="AA100" s="17"/>
+      <c r="AB100" s="17"/>
+      <c r="AC100" s="17"/>
+      <c r="AD100" s="17"/>
+      <c r="AE100" s="17"/>
+      <c r="AF100" s="17"/>
     </row>
     <row r="101" spans="1:32">
       <c r="A101" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="22" t="s">
+      <c r="B101" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="22"/>
-      <c r="D101" s="22"/>
-      <c r="E101" s="22" t="s">
+      <c r="C101" s="17"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F101" s="22"/>
-      <c r="G101" s="22"/>
-      <c r="H101" s="22" t="s">
+      <c r="F101" s="17"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I101" s="22"/>
-      <c r="J101" s="22"/>
+      <c r="I101" s="17"/>
+      <c r="J101" s="17"/>
       <c r="L101" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M101" s="17" t="s">
+      <c r="M101" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="N101" s="18"/>
-      <c r="O101" s="19"/>
-      <c r="P101" s="17" t="s">
+      <c r="N101" s="20"/>
+      <c r="O101" s="21"/>
+      <c r="P101" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="Q101" s="18"/>
-      <c r="R101" s="19"/>
-      <c r="S101" s="22" t="s">
+      <c r="Q101" s="20"/>
+      <c r="R101" s="21"/>
+      <c r="S101" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="T101" s="22"/>
-      <c r="U101" s="22"/>
+      <c r="T101" s="17"/>
+      <c r="U101" s="17"/>
       <c r="W101" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="X101" s="22" t="s">
+      <c r="X101" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="Y101" s="22"/>
-      <c r="Z101" s="22"/>
-      <c r="AA101" s="22" t="s">
+      <c r="Y101" s="17"/>
+      <c r="Z101" s="17"/>
+      <c r="AA101" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="AB101" s="22"/>
-      <c r="AC101" s="22"/>
-      <c r="AD101" s="22" t="s">
+      <c r="AB101" s="17"/>
+      <c r="AC101" s="17"/>
+      <c r="AD101" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="AE101" s="22"/>
-      <c r="AF101" s="22"/>
+      <c r="AE101" s="17"/>
+      <c r="AF101" s="17"/>
     </row>
     <row r="102" spans="1:32">
       <c r="B102" s="1" t="s">
@@ -7304,8 +7349,621 @@
         <v>716</v>
       </c>
     </row>
+    <row r="108" spans="1:32">
+      <c r="B108" t="s">
+        <v>37</v>
+      </c>
+      <c r="F108" t="s">
+        <v>36</v>
+      </c>
+      <c r="J108" t="s">
+        <v>35</v>
+      </c>
+      <c r="N108" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="109" spans="1:32">
+      <c r="A109" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B109" s="26"/>
+      <c r="C109" s="26"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="25"/>
+      <c r="I109" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J109" s="24"/>
+      <c r="K109" s="24"/>
+      <c r="M109" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="N109" s="24"/>
+      <c r="O109" s="24"/>
+    </row>
+    <row r="110" spans="1:32">
+      <c r="A110" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" t="s">
+        <v>28</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
+        <v>28</v>
+      </c>
+      <c r="F110" t="s">
+        <v>26</v>
+      </c>
+      <c r="G110" t="s">
+        <v>1</v>
+      </c>
+      <c r="I110" t="s">
+        <v>28</v>
+      </c>
+      <c r="J110" t="s">
+        <v>26</v>
+      </c>
+      <c r="K110" t="s">
+        <v>1</v>
+      </c>
+      <c r="M110" t="s">
+        <v>28</v>
+      </c>
+      <c r="N110" t="s">
+        <v>26</v>
+      </c>
+      <c r="O110" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:32">
+      <c r="A111">
+        <v>9.77</v>
+      </c>
+      <c r="B111">
+        <v>23.51</v>
+      </c>
+      <c r="C111">
+        <v>3.34</v>
+      </c>
+      <c r="E111">
+        <v>19.84</v>
+      </c>
+      <c r="F111">
+        <v>8.52</v>
+      </c>
+      <c r="G111">
+        <v>4.72</v>
+      </c>
+      <c r="I111">
+        <v>35.24</v>
+      </c>
+      <c r="J111">
+        <v>3.13</v>
+      </c>
+      <c r="K111">
+        <v>3.26</v>
+      </c>
+      <c r="M111">
+        <v>31.53</v>
+      </c>
+      <c r="N111">
+        <v>7.54</v>
+      </c>
+      <c r="O111">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="112" spans="1:32">
+      <c r="A112">
+        <v>6.54</v>
+      </c>
+      <c r="B112">
+        <v>26.61</v>
+      </c>
+      <c r="C112">
+        <v>1.42</v>
+      </c>
+      <c r="E112">
+        <v>13.85</v>
+      </c>
+      <c r="F112">
+        <v>4.82</v>
+      </c>
+      <c r="G112">
+        <v>1.47</v>
+      </c>
+      <c r="I112">
+        <v>32.5</v>
+      </c>
+      <c r="J112">
+        <v>0.68</v>
+      </c>
+      <c r="K112">
+        <v>0.5</v>
+      </c>
+      <c r="M112">
+        <v>22.09</v>
+      </c>
+      <c r="N112">
+        <v>7.31</v>
+      </c>
+      <c r="O112">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
+      <c r="A113">
+        <v>6.57</v>
+      </c>
+      <c r="B113">
+        <v>26.19</v>
+      </c>
+      <c r="C113">
+        <v>1.53</v>
+      </c>
+      <c r="E113">
+        <v>18.98</v>
+      </c>
+      <c r="F113">
+        <v>5.37</v>
+      </c>
+      <c r="G113">
+        <v>1.66</v>
+      </c>
+      <c r="I113">
+        <v>29.67</v>
+      </c>
+      <c r="J113">
+        <v>0.6</v>
+      </c>
+      <c r="K113">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M113">
+        <v>20.38</v>
+      </c>
+      <c r="N113">
+        <v>7.26</v>
+      </c>
+      <c r="O113">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15">
+      <c r="A114">
+        <v>6.78</v>
+      </c>
+      <c r="B114">
+        <v>26.48</v>
+      </c>
+      <c r="C114">
+        <v>1.43</v>
+      </c>
+      <c r="E114">
+        <v>13.98</v>
+      </c>
+      <c r="F114">
+        <v>4.82</v>
+      </c>
+      <c r="G114">
+        <v>1.46</v>
+      </c>
+      <c r="I114">
+        <v>29.02</v>
+      </c>
+      <c r="J114">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K114">
+        <v>0.48</v>
+      </c>
+      <c r="M114">
+        <v>22.54</v>
+      </c>
+      <c r="N114">
+        <v>7.3</v>
+      </c>
+      <c r="O114">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15">
+      <c r="A115">
+        <v>6.64</v>
+      </c>
+      <c r="B115">
+        <v>23.13</v>
+      </c>
+      <c r="C115">
+        <v>1.41</v>
+      </c>
+      <c r="E115">
+        <v>13.9</v>
+      </c>
+      <c r="F115">
+        <v>4.84</v>
+      </c>
+      <c r="G115">
+        <v>1.46</v>
+      </c>
+      <c r="I115">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="J115">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K115">
+        <v>0.34</v>
+      </c>
+      <c r="M115">
+        <v>20.76</v>
+      </c>
+      <c r="N115">
+        <v>7.7</v>
+      </c>
+      <c r="O115">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
+      <c r="A116">
+        <v>8.74</v>
+      </c>
+      <c r="B116">
+        <v>25.8</v>
+      </c>
+      <c r="C116">
+        <v>1.41</v>
+      </c>
+      <c r="E116">
+        <v>14.35</v>
+      </c>
+      <c r="F116">
+        <v>5.49</v>
+      </c>
+      <c r="G116">
+        <v>1.67</v>
+      </c>
+      <c r="I116">
+        <v>34.94</v>
+      </c>
+      <c r="J116">
+        <v>0.3</v>
+      </c>
+      <c r="K116">
+        <v>0.46</v>
+      </c>
+      <c r="M116">
+        <v>22.6</v>
+      </c>
+      <c r="N116">
+        <v>7.68</v>
+      </c>
+      <c r="O116">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15">
+      <c r="A117">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="B117">
+        <v>26.3</v>
+      </c>
+      <c r="C117">
+        <v>1.41</v>
+      </c>
+      <c r="E117">
+        <v>14.28</v>
+      </c>
+      <c r="F117">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="G117">
+        <v>1.62</v>
+      </c>
+      <c r="I117">
+        <v>35.5</v>
+      </c>
+      <c r="J117">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K117">
+        <v>0.47</v>
+      </c>
+      <c r="M117">
+        <v>26.99</v>
+      </c>
+      <c r="N117">
+        <v>7.56</v>
+      </c>
+      <c r="O117">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15">
+      <c r="A118">
+        <v>5.13</v>
+      </c>
+      <c r="B118">
+        <v>25.84</v>
+      </c>
+      <c r="C118">
+        <v>1.41</v>
+      </c>
+      <c r="E118">
+        <v>13.93</v>
+      </c>
+      <c r="F118">
+        <v>9.74</v>
+      </c>
+      <c r="G118">
+        <v>1.03</v>
+      </c>
+      <c r="I118">
+        <v>39.22</v>
+      </c>
+      <c r="J118">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K118">
+        <v>0.46</v>
+      </c>
+      <c r="M118">
+        <v>22.34</v>
+      </c>
+      <c r="N118">
+        <v>7.44</v>
+      </c>
+      <c r="O118">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15">
+      <c r="A119">
+        <v>6.86</v>
+      </c>
+      <c r="B119">
+        <v>25.94</v>
+      </c>
+      <c r="C119">
+        <v>1.82</v>
+      </c>
+      <c r="E119">
+        <v>14.45</v>
+      </c>
+      <c r="F119">
+        <v>4.82</v>
+      </c>
+      <c r="G119">
+        <v>6.25</v>
+      </c>
+      <c r="I119">
+        <v>29.43</v>
+      </c>
+      <c r="J119">
+        <v>0.59</v>
+      </c>
+      <c r="K119">
+        <v>0.48</v>
+      </c>
+      <c r="M119">
+        <v>26.96</v>
+      </c>
+      <c r="N119">
+        <v>7.61</v>
+      </c>
+      <c r="O119">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15">
+      <c r="A120">
+        <v>6.95</v>
+      </c>
+      <c r="B120">
+        <v>25.95</v>
+      </c>
+      <c r="C120">
+        <v>1.05</v>
+      </c>
+      <c r="E120">
+        <v>19.41</v>
+      </c>
+      <c r="F120">
+        <v>3.41</v>
+      </c>
+      <c r="G120">
+        <v>1.59</v>
+      </c>
+      <c r="I120">
+        <v>34.65</v>
+      </c>
+      <c r="J120">
+        <v>0.37</v>
+      </c>
+      <c r="K120">
+        <v>0.35</v>
+      </c>
+      <c r="M120">
+        <v>22.57</v>
+      </c>
+      <c r="N120">
+        <v>7.44</v>
+      </c>
+      <c r="O120">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15">
+      <c r="A121" s="27">
+        <f>AVERAGE(A111:A120)</f>
+        <v>6.8840000000000003</v>
+      </c>
+      <c r="B121" s="27">
+        <f>AVERAGE(B111:B120)</f>
+        <v>25.574999999999999</v>
+      </c>
+      <c r="C121" s="27">
+        <f>AVERAGE(C111:C120)</f>
+        <v>1.623</v>
+      </c>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27">
+        <f t="shared" ref="D121:G121" si="12">AVERAGE(E111:E120)</f>
+        <v>15.696999999999999</v>
+      </c>
+      <c r="F121" s="27">
+        <f t="shared" si="12"/>
+        <v>5.6639999999999997</v>
+      </c>
+      <c r="G121" s="27">
+        <f t="shared" si="12"/>
+        <v>2.2929999999999997</v>
+      </c>
+      <c r="H121" s="27"/>
+      <c r="I121" s="27">
+        <f t="shared" ref="I121" si="13">AVERAGE(I111:I120)</f>
+        <v>33.346999999999994</v>
+      </c>
+      <c r="J121" s="27">
+        <f t="shared" ref="J121" si="14">AVERAGE(J111:J120)</f>
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="K121" s="27">
+        <f>AVERAGE(K111:K120)</f>
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="L121" s="27"/>
+      <c r="M121" s="27">
+        <f t="shared" ref="M121" si="15">AVERAGE(M111:M120)</f>
+        <v>23.876000000000001</v>
+      </c>
+      <c r="N121" s="27">
+        <f t="shared" ref="N121" si="16">AVERAGE(N111:N120)</f>
+        <v>7.484</v>
+      </c>
+      <c r="O121" s="27">
+        <f t="shared" ref="O121" si="17">AVERAGE(O111:O120)</f>
+        <v>2.726</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="124">
+  <mergeCells count="128">
+    <mergeCell ref="A109:C109"/>
+    <mergeCell ref="E109:G109"/>
+    <mergeCell ref="I109:K109"/>
+    <mergeCell ref="M109:O109"/>
+    <mergeCell ref="X4:AF4"/>
+    <mergeCell ref="X5:AF5"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AC6"/>
+    <mergeCell ref="AD6:AF6"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="M4:U4"/>
+    <mergeCell ref="M5:U5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="P6:R6"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="M22:U22"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="X22:AF22"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="B50:J50"/>
+    <mergeCell ref="X23:AF23"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="M31:U31"/>
+    <mergeCell ref="A28:AF29"/>
+    <mergeCell ref="M23:U23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="M32:U32"/>
+    <mergeCell ref="X24:Z24"/>
+    <mergeCell ref="AA24:AC24"/>
+    <mergeCell ref="AD24:AF24"/>
+    <mergeCell ref="M49:U49"/>
+    <mergeCell ref="X31:AF31"/>
+    <mergeCell ref="X32:AF32"/>
+    <mergeCell ref="X33:Z33"/>
+    <mergeCell ref="AA33:AC33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="S33:U33"/>
+    <mergeCell ref="A55:AF56"/>
+    <mergeCell ref="B58:J58"/>
+    <mergeCell ref="B59:J59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="H60:J60"/>
+    <mergeCell ref="AD33:AF33"/>
+    <mergeCell ref="X49:AF49"/>
+    <mergeCell ref="X50:AF50"/>
+    <mergeCell ref="X51:Z51"/>
+    <mergeCell ref="AA51:AC51"/>
+    <mergeCell ref="AD51:AF51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="M50:U50"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="S51:U51"/>
+    <mergeCell ref="X58:AF58"/>
+    <mergeCell ref="X59:AF59"/>
+    <mergeCell ref="X60:Z60"/>
+    <mergeCell ref="AA60:AC60"/>
+    <mergeCell ref="AD60:AF60"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="B75:J75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="H76:J76"/>
+    <mergeCell ref="M58:U58"/>
+    <mergeCell ref="M59:U59"/>
+    <mergeCell ref="M60:O60"/>
+    <mergeCell ref="P60:R60"/>
+    <mergeCell ref="S60:U60"/>
+    <mergeCell ref="M100:U100"/>
+    <mergeCell ref="B84:J84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="H85:J85"/>
+    <mergeCell ref="B99:J99"/>
+    <mergeCell ref="B100:J100"/>
+    <mergeCell ref="X74:AF74"/>
+    <mergeCell ref="X75:AF75"/>
+    <mergeCell ref="X76:Z76"/>
+    <mergeCell ref="AA76:AC76"/>
+    <mergeCell ref="AD76:AF76"/>
+    <mergeCell ref="B83:J83"/>
+    <mergeCell ref="M74:U74"/>
+    <mergeCell ref="M75:U75"/>
+    <mergeCell ref="M76:O76"/>
+    <mergeCell ref="P76:R76"/>
+    <mergeCell ref="S76:U76"/>
     <mergeCell ref="X101:Z101"/>
     <mergeCell ref="AA101:AC101"/>
     <mergeCell ref="AD101:AF101"/>
@@ -7330,106 +7988,6 @@
     <mergeCell ref="P85:R85"/>
     <mergeCell ref="S85:U85"/>
     <mergeCell ref="M99:U99"/>
-    <mergeCell ref="M100:U100"/>
-    <mergeCell ref="B84:J84"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="H85:J85"/>
-    <mergeCell ref="B99:J99"/>
-    <mergeCell ref="B100:J100"/>
-    <mergeCell ref="X74:AF74"/>
-    <mergeCell ref="X75:AF75"/>
-    <mergeCell ref="X76:Z76"/>
-    <mergeCell ref="AA76:AC76"/>
-    <mergeCell ref="AD76:AF76"/>
-    <mergeCell ref="B83:J83"/>
-    <mergeCell ref="M74:U74"/>
-    <mergeCell ref="M75:U75"/>
-    <mergeCell ref="M76:O76"/>
-    <mergeCell ref="P76:R76"/>
-    <mergeCell ref="S76:U76"/>
-    <mergeCell ref="AA60:AC60"/>
-    <mergeCell ref="AD60:AF60"/>
-    <mergeCell ref="B74:J74"/>
-    <mergeCell ref="B75:J75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="H76:J76"/>
-    <mergeCell ref="M58:U58"/>
-    <mergeCell ref="M59:U59"/>
-    <mergeCell ref="M60:O60"/>
-    <mergeCell ref="P60:R60"/>
-    <mergeCell ref="S60:U60"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="S33:U33"/>
-    <mergeCell ref="A55:AF56"/>
-    <mergeCell ref="B58:J58"/>
-    <mergeCell ref="B59:J59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="H60:J60"/>
-    <mergeCell ref="AD33:AF33"/>
-    <mergeCell ref="X49:AF49"/>
-    <mergeCell ref="X50:AF50"/>
-    <mergeCell ref="X51:Z51"/>
-    <mergeCell ref="AA51:AC51"/>
-    <mergeCell ref="AD51:AF51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="M50:U50"/>
-    <mergeCell ref="M51:O51"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="S51:U51"/>
-    <mergeCell ref="X58:AF58"/>
-    <mergeCell ref="X59:AF59"/>
-    <mergeCell ref="X60:Z60"/>
-    <mergeCell ref="B32:J32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="B50:J50"/>
-    <mergeCell ref="X23:AF23"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="M31:U31"/>
-    <mergeCell ref="A28:AF29"/>
-    <mergeCell ref="M23:U23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="M32:U32"/>
-    <mergeCell ref="X24:Z24"/>
-    <mergeCell ref="AA24:AC24"/>
-    <mergeCell ref="AD24:AF24"/>
-    <mergeCell ref="M49:U49"/>
-    <mergeCell ref="X31:AF31"/>
-    <mergeCell ref="X32:AF32"/>
-    <mergeCell ref="X33:Z33"/>
-    <mergeCell ref="AA33:AC33"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="X4:AF4"/>
-    <mergeCell ref="X5:AF5"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AC6"/>
-    <mergeCell ref="AD6:AF6"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="M4:U4"/>
-    <mergeCell ref="M5:U5"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="P6:R6"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="M22:U22"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="X22:AF22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>